<commit_message>
adding plan formulation - test
</commit_message>
<xml_diff>
--- a/Final Deliverables/Final_Cleaned_DataFrame.xlsx
+++ b/Final Deliverables/Final_Cleaned_DataFrame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Food Truck</t>
+          <t>Food_Truck</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Phone Number</t>
+          <t>Phone_Number</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -461,64 +461,72 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Review_Count</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Operating Hours</t>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Operating_Hours</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The Legendary Kitchen</t>
+          <t>The Alkaline Electric Goddess</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/the-legendary-kitchen-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/the-alkaline-electric-goddess-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(800) 568-9370</t>
+          <t>(317) 662-4498</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Food Trucks</t>
+          <t>Health Markets</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>40 E St Clair St, Indianapolis, IN 46204, USA</t>
-        </is>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>09:00 AM - 05:00 PM</t>
+          <t>49 W Maryland St unit 118a, Indianapolis, IN 46204, USA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>05:00 PM - 09:00 PM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ice Cream On Wheels</t>
+          <t>The Legendary Kitchen</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/ice-cream-on-wheels-indianapolis-6?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/the-legendary-kitchen-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(800) 884-9793</t>
+          <t>(800) 568-9370</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -529,136 +537,148 @@
       <c r="E3" t="n">
         <v>5</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>4215 W Thompson Rd, Indianapolis, IN 46221, USA</t>
-        </is>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>12:00 AM - 12:00 AM</t>
+          <t>40 E St Clair St, Indianapolis, IN 46204, USA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>09:00 AM - 05:00 PM</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Traveling Taste Buds</t>
+          <t>La Familia</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/traveling-taste-buds-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/la-familia-food-truck-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(317) 531-6155</t>
+          <t>(463) 280-4499</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Food Trucks</t>
+          <t>Tacos</t>
         </is>
       </c>
       <c r="E4" t="n">
         <v>5</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1 Monument Cir, Indianapolis, IN 46204, USA</t>
-        </is>
+      <c r="F4" t="n">
+        <v>8</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>12:00 AM - 12:00 AM</t>
+          <t>311 Troy Ct, Indianapolis, IN 46227, USA</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>11:00 AM - 11:00 PM</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HomeTeam Ice Cream</t>
+          <t>Tapatia Mexican Tacos</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/hometeam-ice-cream-kokomo?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/tapatia-mexican-tacos-warren-park?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(765) 437-6843</t>
+          <t>(317) 490-2417</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Food Trucks</t>
+          <t>Tacos</t>
         </is>
       </c>
       <c r="E5" t="n">
         <v>5</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>709 N Union St, Kokomo, IN 46901, USA</t>
-        </is>
+      <c r="F5" t="n">
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>04:00 PM - 08:00 PM</t>
+          <t>7202 E Washington St, Indianapolis, IN 46219, USA</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>12:00 PM - 11:00 PM</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tacopolis</t>
+          <t>Traveling Taste Buds</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/tacopolis-indianapolis-2?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/traveling-taste-buds-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(317) 488-8724</t>
+          <t>(317) 531-6155</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Tacos</t>
+          <t>Food Trucks</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>5</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>4857 W 38th St, Indianapolis, IN 46254, USA</t>
-        </is>
+      <c r="F6" t="n">
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>02:00 PM - 11:30 PM</t>
+          <t>1 Monument Cir, Indianapolis, IN 46204, USA</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>12:00 AM - 12:00 AM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TACO LOCO M&amp;C</t>
+          <t>HomeTeam Ice Cream</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/taco-loco-m-and-c-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/hometeam-ice-cream-kokomo?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(463) 210-9667</t>
+          <t>(765) 437-6843</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -669,66 +689,72 @@
       <c r="E7" t="n">
         <v>5</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>1415 W 86th St, Indianapolis, IN 46260, USA</t>
-        </is>
+      <c r="F7" t="n">
+        <v>2</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>06:00 PM - 12:00 AM</t>
+          <t>709 N Union St, Kokomo, IN 46901, USA</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>04:00 PM - 08:00 PM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tapatia Mexican Tacos</t>
+          <t>Ice Cream On Wheels</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/tapatia-mexican-tacos-warren-park?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/ice-cream-on-wheels-indianapolis-6?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(317) 490-2417</t>
+          <t>(800) 884-9793</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Tacos</t>
+          <t>Food Trucks</t>
         </is>
       </c>
       <c r="E8" t="n">
         <v>5</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>7202 E Washington St, Indianapolis, IN 46219, USA</t>
-        </is>
+      <c r="F8" t="n">
+        <v>1</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>12:00 PM - 11:00 PM</t>
+          <t>4215 W Thompson Rd, Indianapolis, IN 46221, USA</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>12:00 AM - 12:00 AM</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>La Familia</t>
+          <t>Tacopolis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/la-familia-food-truck-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/tacopolis-indianapolis-2?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>(463) 280-4499</t>
+          <t>(317) 488-8724</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -739,49 +765,55 @@
       <c r="E9" t="n">
         <v>5</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>311 Troy Ct, Indianapolis, IN 46227, USA</t>
-        </is>
+      <c r="F9" t="n">
+        <v>5</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>11:00 AM - 11:00 PM</t>
+          <t>4857 W 38th St, Indianapolis, IN 46254, USA</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>02:00 PM - 11:30 PM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BB&amp;B Bread Truck</t>
+          <t>TACO LOCO M&amp;C</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/bb-and-b-bread-truck-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/taco-loco-m-and-c-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>(317) 730-4778</t>
+          <t>(463) 210-9667</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bakeries</t>
+          <t>Food Trucks</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>800 Lafayette St, Indianapolis, IN 46202, USA</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>05:00 PM - 10:00 PM</t>
+          <t>1415 W 86th St, Indianapolis, IN 46260, USA</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>06:00 PM - 12:00 AM</t>
         </is>
       </c>
     </row>
@@ -809,12 +841,15 @@
       <c r="E11" t="n">
         <v>4.5</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>19</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>8375 Allison Pointe Blvd, Indianapolis, IN 46250, USA</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>06:30 AM - 08:00 PM</t>
         </is>
@@ -844,12 +879,15 @@
       <c r="E12" t="n">
         <v>4.5</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>4202 W 56th St, Indianapolis, IN 46254, USA</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>05:00 AM - 01:00 PM</t>
         </is>
@@ -879,12 +917,15 @@
       <c r="E13" t="n">
         <v>4.5</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>3633 Kentucky Ave, Indianapolis, IN 46221, USA</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>11:00 AM - 07:45 PM</t>
         </is>
@@ -893,103 +934,112 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Taste of Cholulas</t>
+          <t>BB&amp;B Bread Truck</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/taste-of-cholulas-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/bb-and-b-bread-truck-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>(317) 628-1258</t>
+          <t>(317) 730-4778</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Tacos</t>
+          <t>Bakeries</t>
         </is>
       </c>
       <c r="E14" t="n">
         <v>4.5</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>8901-8925 E Washington St, Indianapolis, IN 46219, USA</t>
-        </is>
+      <c r="F14" t="n">
+        <v>38</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>05:00 PM - 12:00 AM</t>
+          <t>800 Lafayette St, Indianapolis, IN 46202, USA</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>05:00 PM - 10:00 PM</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Big Reds Bbq Food Truck</t>
+          <t>Taqueria Oaxaca Indy</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/big-reds-bbq-food-truck-shelbyville?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/taqueria-oaxaca-indy-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>(513) 256-8052</t>
+          <t>(317) 490-2429</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Barbeque</t>
+          <t>Mexican</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v>4.5</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>408 S Harrison St, Shelbyville, IN 46176, USA</t>
-        </is>
+      <c r="F15" t="n">
+        <v>9</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>06:00 PM - 09:00 PM</t>
+          <t>4501 W 38th St, Indianapolis, IN 46254, USA</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>07:00 PM - 01:00 AM</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Taqueria Oaxaca Indy</t>
+          <t>Fast Taco's</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/taqueria-oaxaca-indy-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/fast-tacos-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>(317) 490-2429</t>
+          <t>(317) 701-8182</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Mexican</t>
+          <t>Food Trucks</t>
         </is>
       </c>
       <c r="E16" t="n">
         <v>4.5</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>4501 W 38th St, Indianapolis, IN 46254, USA</t>
-        </is>
+      <c r="F16" t="n">
+        <v>16</v>
       </c>
       <c r="G16" t="inlineStr">
+        <is>
+          <t>6154 Michigan Rd, Indianapolis, IN 46228, USA</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>07:00 PM - 01:00 AM</t>
         </is>
@@ -998,175 +1048,190 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Fast Taco's</t>
+          <t>Serendipity Mobile Catering</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/fast-tacos-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/serendipity-mobile-catering-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>(317) 701-8182</t>
+          <t>(317) 306-6870</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Food Trucks</t>
+          <t>Caterers</t>
         </is>
       </c>
       <c r="E17" t="n">
         <v>4.5</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>6154 Michigan Rd, Indianapolis, IN 46228, USA</t>
-        </is>
+      <c r="F17" t="n">
+        <v>32</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>07:00 PM - 01:00 AM</t>
+          <t>5922 N College Ave, Indianapolis, IN 46220, USA</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>07:00 AM - 01:00 AM</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Serendipity Mobile Catering</t>
+          <t>Birrieria Iturbidense</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/serendipity-mobile-catering-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/birrieria-iturbidense-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>(317) 306-6870</t>
+          <t>(317) 828-3558</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Caterers</t>
+          <t>Tacos</t>
         </is>
       </c>
       <c r="E18" t="n">
         <v>4.5</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>5922 N College Ave, Indianapolis, IN 46220, USA</t>
-        </is>
+      <c r="F18" t="n">
+        <v>40</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>07:00 AM - 01:00 AM</t>
+          <t>6302 W Washington St, Indianapolis, IN 46241, USA</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>06:00 PM - 12:00 AM</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Birrieria Iturbidense</t>
+          <t>Gaucho's Fire Express</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/birrieria-iturbidense-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/gauchos-fire-express-indianapolis-2?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>(317) 828-3558</t>
+          <t>(317) 344-9921</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Tacos</t>
+          <t>Caterers</t>
         </is>
       </c>
       <c r="E19" t="n">
         <v>4.5</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>6302 W Washington St, Indianapolis, IN 46241, USA</t>
-        </is>
+      <c r="F19" t="n">
+        <v>77</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>06:00 PM - 12:00 AM</t>
+          <t>1280 N Senate Ave, Indianapolis, IN 46202, USA</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>10:30 AM - 09:00 PM</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Gaucho's Fire Express</t>
+          <t>Big Reds Bbq Food Truck</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/gauchos-fire-express-indianapolis-2?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/big-reds-bbq-food-truck-shelbyville?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>(317) 344-9921</t>
+          <t>(513) 256-8052</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Caterers</t>
+          <t>Barbeque</t>
         </is>
       </c>
       <c r="E20" t="n">
         <v>4.5</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>1280 N Senate Ave, Indianapolis, IN 46202, USA</t>
-        </is>
+      <c r="F20" t="n">
+        <v>2</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>10:30 AM - 09:00 PM</t>
+          <t>408 S Harrison St, Shelbyville, IN 46176, USA</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>06:00 PM - 09:00 PM</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Pi Indy</t>
+          <t>Black Leaf Vegan</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/pi-indy-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/black-leaf-vegan-indianapolis-2?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>(317) 903-2612</t>
+          <t>(317) 560-4222</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Pizza</t>
+          <t>Comfort Food</t>
         </is>
       </c>
       <c r="E21" t="n">
         <v>4</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>8222 Indy Ln, Indianapolis, IN 46214, USA</t>
-        </is>
+      <c r="F21" t="n">
+        <v>65</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>05:00 PM - 08:00 PM</t>
+          <t>335 W 9th St, Indianapolis, IN 46202, USA</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>08:00 AM - 06:00 PM</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1259,15 @@
       <c r="E22" t="n">
         <v>4</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>7210 N Michigan Rd, Indianapolis, IN 46268, USA</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>11:00 AM - 09:00 PM</t>
         </is>
@@ -1208,35 +1276,38 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Poccadio Grill Food Truck</t>
+          <t>Pi Indy</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/poccadio-grill-food-truck-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/pi-indy-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>(317) 252-5911</t>
+          <t>(317) 903-2612</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Food Trucks</t>
+          <t>Pizza</t>
         </is>
       </c>
       <c r="E23" t="n">
         <v>4</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>6116 N Chester Ave, Indianapolis, IN 46220, USA</t>
-        </is>
+      <c r="F23" t="n">
+        <v>36</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>11:00 AM - 11:00 PM</t>
+          <t>8222 Indy Ln, Indianapolis, IN 46214, USA</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>05:00 PM - 08:00 PM</t>
         </is>
       </c>
     </row>
@@ -1264,12 +1335,15 @@
       <c r="E24" t="n">
         <v>4</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>901 Broad Ripple Ave, Indianapolis, IN 46220, USA</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>10:00 AM - 09:00 PM</t>
         </is>
@@ -1278,35 +1352,38 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Black Leaf Vegan</t>
+          <t>Poccadio Grill Food Truck</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.yelp.com/biz/black-leaf-vegan-indianapolis-2?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
+          <t>https://www.yelp.com/biz/poccadio-grill-food-truck-indianapolis?adjust_creative=7dFhg7WTQv5IwbOVO9QLzw&amp;utm_campaign=yelp_api_v3&amp;utm_medium=api_v3_business_lookup&amp;utm_source=7dFhg7WTQv5IwbOVO9QLzw</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>(317) 560-4222</t>
+          <t>(317) 252-5911</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Comfort Food</t>
+          <t>Food Trucks</t>
         </is>
       </c>
       <c r="E25" t="n">
         <v>4</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>335 W 9th St, Indianapolis, IN 46202, USA</t>
-        </is>
+      <c r="F25" t="n">
+        <v>13</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>08:00 AM - 06:00 PM</t>
+          <t>6116 N Chester Ave, Indianapolis, IN 46220, USA</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>11:00 AM - 11:00 PM</t>
         </is>
       </c>
     </row>
@@ -1334,12 +1411,15 @@
       <c r="E26" t="n">
         <v>3.5</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="n">
+        <v>118</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>2126 Shelby St, Indianapolis, IN 46203, USA</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>10:30 AM - 08:00 PM</t>
         </is>
@@ -1369,12 +1449,15 @@
       <c r="E27" t="n">
         <v>3.5</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="n">
+        <v>17</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>2073 N Emerson Ave, Indianapolis, IN 46218, USA</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>12:00 PM - 08:00 PM</t>
         </is>
@@ -1404,12 +1487,15 @@
       <c r="E28" t="n">
         <v>3</v>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="n">
+        <v>18</v>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>336 N Riley Ave, Indianapolis, IN 46201, USA</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>11:00 AM - 01:30 PM</t>
         </is>
@@ -1439,12 +1525,15 @@
       <c r="E29" t="n">
         <v>2.5</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>2537 E 38th St, Indianapolis, IN 46218, USA</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>04:00 PM - 11:00 PM</t>
         </is>

</xml_diff>